<commit_message>
Finalize descriptive analysis for a continuous and categorical outcome variable
</commit_message>
<xml_diff>
--- a/documentation/Categorical_Tbl 1_Blank.xlsx
+++ b/documentation/Categorical_Tbl 1_Blank.xlsx
@@ -1,20 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Dropbox\Monika!\BRFSS Descriptive\Chapter 5-Conducting Descriptive Analysis\Sect 1-Preparing Categorical Table 1 shell\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RProjects\github\BRFSS\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A300A137-E3D0-4E22-84B0-10F2ADBF96D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="48" windowWidth="17232" windowHeight="8016"/>
+    <workbookView xWindow="17310" yWindow="-14685" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1 Categorical" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -267,7 +275,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -700,32 +708,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" style="1"/>
-    <col min="8" max="8" width="9.109375" style="5"/>
-    <col min="9" max="9" width="10.33203125" style="9" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" style="1"/>
-    <col min="11" max="11" width="10.33203125" style="9" customWidth="1"/>
-    <col min="12" max="12" width="9.109375" style="10"/>
-    <col min="13" max="13" width="10.33203125" style="9" customWidth="1"/>
-    <col min="14" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="9.140625" style="5"/>
+    <col min="9" max="9" width="10.28515625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="1"/>
+    <col min="11" max="11" width="10.28515625" style="9" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="10"/>
+    <col min="13" max="13" width="10.28515625" style="9" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="4" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -775,7 +783,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -818,7 +826,7 @@
         <v>52788</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -853,7 +861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>32</v>
       </c>
@@ -885,7 +893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
@@ -917,7 +925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -952,7 +960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>34</v>
       </c>
@@ -984,7 +992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>35</v>
       </c>
@@ -1016,7 +1024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>36</v>
       </c>
@@ -1048,7 +1056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>37</v>
       </c>
@@ -1080,7 +1088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>38</v>
       </c>
@@ -1112,7 +1120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>39</v>
       </c>
@@ -1147,7 +1155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
@@ -1179,7 +1187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>41</v>
       </c>
@@ -1214,7 +1222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>42</v>
       </c>
@@ -1246,7 +1254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>11</v>
       </c>
@@ -1278,7 +1286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
@@ -1313,7 +1321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>44</v>
       </c>
@@ -1345,7 +1353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>46</v>
       </c>
@@ -1377,7 +1385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>45</v>
       </c>
@@ -1409,7 +1417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>75</v>
       </c>
@@ -1441,7 +1449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>8</v>
       </c>
@@ -1473,7 +1481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>11</v>
       </c>
@@ -1505,7 +1513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>58</v>
       </c>
@@ -1540,7 +1548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>60</v>
       </c>
@@ -1572,7 +1580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>61</v>
       </c>
@@ -1604,7 +1612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
@@ -1636,7 +1644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>78</v>
       </c>
@@ -1671,7 +1679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>77</v>
       </c>
@@ -1703,7 +1711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>9</v>
       </c>
@@ -1735,7 +1743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>10</v>
       </c>
@@ -1767,7 +1775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>11</v>
       </c>
@@ -1799,7 +1807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>79</v>
       </c>
@@ -1834,7 +1842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>51</v>
       </c>
@@ -1866,7 +1874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>52</v>
       </c>
@@ -1898,7 +1906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>53</v>
       </c>
@@ -1930,7 +1938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>54</v>
       </c>
@@ -1962,7 +1970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>55</v>
       </c>
@@ -1994,7 +2002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>56</v>
       </c>
@@ -2026,7 +2034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>57</v>
       </c>
@@ -2058,7 +2066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
         <v>11</v>
       </c>
@@ -2090,7 +2098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>12</v>
       </c>
@@ -2125,7 +2133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>14</v>
       </c>
@@ -2157,7 +2165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
         <v>15</v>
       </c>
@@ -2189,7 +2197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
         <v>16</v>
       </c>
@@ -2221,7 +2229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
         <v>11</v>
       </c>
@@ -2253,7 +2261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>17</v>
       </c>
@@ -2288,7 +2296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
         <v>19</v>
       </c>
@@ -2320,7 +2328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
         <v>11</v>
       </c>
@@ -2352,7 +2360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>21</v>
       </c>
@@ -2387,7 +2395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
         <v>23</v>
       </c>
@@ -2419,7 +2427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
         <v>11</v>
       </c>
@@ -2451,7 +2459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>47</v>
       </c>
@@ -2486,7 +2494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
         <v>49</v>
       </c>
@@ -2518,7 +2526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B55" s="1" t="s">
         <v>11</v>
       </c>
@@ -2550,7 +2558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>24</v>
       </c>
@@ -2585,7 +2593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B57" s="1" t="s">
         <v>26</v>
       </c>
@@ -2617,7 +2625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B58" s="1" t="s">
         <v>27</v>
       </c>
@@ -2649,7 +2657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B59" s="1" t="s">
         <v>28</v>
       </c>
@@ -2681,7 +2689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B60" s="1" t="s">
         <v>29</v>
       </c>
@@ -2713,7 +2721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B61" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>